<commit_message>
Basic data validations for numeric values are available. Also some sort of list validations are working.
</commit_message>
<xml_diff>
--- a/DataValidation/test-files/DataValidationTest.xlsx
+++ b/DataValidation/test-files/DataValidationTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="20400" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -15,15 +15,191 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+  <si>
+    <t>Any Value</t>
+  </si>
+  <si>
+    <t>Case 1</t>
+  </si>
+  <si>
+    <t>Case 2</t>
+  </si>
+  <si>
+    <t>Case 3</t>
+  </si>
+  <si>
+    <t>Case 4</t>
+  </si>
+  <si>
+    <t>Case 5</t>
+  </si>
+  <si>
+    <t>Case 6</t>
+  </si>
+  <si>
+    <t>Case 7</t>
+  </si>
+  <si>
+    <t>Case 8</t>
+  </si>
+  <si>
+    <t>Case 9</t>
+  </si>
+  <si>
+    <t>Case 10</t>
+  </si>
+  <si>
+    <t>Case 11</t>
+  </si>
+  <si>
+    <t>Case 12</t>
+  </si>
+  <si>
+    <t>Case 13</t>
+  </si>
+  <si>
+    <t>Case 14</t>
+  </si>
+  <si>
+    <t>Case 15</t>
+  </si>
+  <si>
+    <t>Case 16</t>
+  </si>
+  <si>
+    <t>Case 17</t>
+  </si>
+  <si>
+    <t>Case 18</t>
+  </si>
+  <si>
+    <t>Whole Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Between </t>
+  </si>
+  <si>
+    <t>Not Between</t>
+  </si>
+  <si>
+    <t>Equal To</t>
+  </si>
+  <si>
+    <t>Not Equal To</t>
+  </si>
+  <si>
+    <t>Greater Than</t>
+  </si>
+  <si>
+    <t>Less Than</t>
+  </si>
+  <si>
+    <t>Less Than Or Equal To</t>
+  </si>
+  <si>
+    <t>Greater Than Or Equal To</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Ahmet, Mehmet, Süleyman</t>
+  </si>
+  <si>
+    <t>Case 20</t>
+  </si>
+  <si>
+    <t>Case 21</t>
+  </si>
+  <si>
+    <t>Case 33</t>
+  </si>
+  <si>
+    <t>Case 35</t>
+  </si>
+  <si>
+    <t>Case 36</t>
+  </si>
+  <si>
+    <t>Case 37</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ref1</t>
+  </si>
+  <si>
+    <t>Ref2</t>
+  </si>
+  <si>
+    <t>Ref3</t>
+  </si>
+  <si>
+    <t>RefS1</t>
+  </si>
+  <si>
+    <t>RefS2</t>
+  </si>
+  <si>
+    <t>RefS3</t>
+  </si>
+  <si>
+    <t>I1:I3</t>
+  </si>
+  <si>
+    <t>Sheet2# C1:C3</t>
+  </si>
+  <si>
+    <t>Ref4!</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Case 38</t>
+  </si>
+  <si>
+    <t>Case 39</t>
+  </si>
+  <si>
+    <t>Case 40</t>
+  </si>
+  <si>
+    <t>Case 41</t>
+  </si>
+  <si>
+    <t>Yusuf</t>
+  </si>
+  <si>
+    <t>RefS4!</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -47,14 +223,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -350,24 +530,689 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1">
+        <v>12</v>
+      </c>
+      <c r="K1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L1" s="1">
+        <v>42343</v>
+      </c>
+      <c r="M1" s="1">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2">
+        <v>14</v>
+      </c>
+      <c r="K2">
+        <v>12.12</v>
+      </c>
+      <c r="L2" s="1">
+        <v>42709</v>
+      </c>
+      <c r="M2" s="1">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>123.123</v>
+      </c>
+      <c r="L3" s="1">
+        <v>43074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>888</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>888</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F10">
+        <v>1.123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>2.21</v>
+      </c>
+      <c r="F11">
+        <v>2.222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>6.66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <v>8.8879999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>1000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2">
+        <v>42005</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>42343</v>
+      </c>
+      <c r="F21" s="2">
+        <v>42710</v>
+      </c>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2">
+        <v>42343</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2">
+        <v>42343</v>
+      </c>
+      <c r="F22" s="2">
+        <v>42710</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2">
+        <v>42370</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2">
+        <v>42343</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2">
+        <v>42343</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2">
+        <v>42343</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2">
+        <v>42370</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2">
+        <v>42340</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="2">
+        <v>42343</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2">
+        <v>42370</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="25">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>1</formula1>
+      <formula2>15</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>5</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>6</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>7</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+      <formula1>65</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>98</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+      <formula1>1.12</formula1>
+      <formula2>1.123</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>2.21</formula1>
+      <formula2>2.222</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+      <formula1>5.55</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
+      <formula1>6.66</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
+      <formula1>8.888</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>888</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+      <formula1>2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+      <formula1>9.9</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
+      <formula1>"Ahmet,Mehmet,Süleyman"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
+      <formula1>$I$1:$I$3</formula1>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+      <formula1>42343</formula1>
+      <formula2>42710</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+      <formula1>42343</formula1>
+      <formula2>42710</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
+      <formula1>42343</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B25">
+      <formula1>42343</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
+      <formula1>42343</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
+      <formula1>42343</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+      <formula1>42343</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>111</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sayfa2!$C$1:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New end-to-end test cases are written
</commit_message>
<xml_diff>
--- a/DataValidation/test-files/DataValidationTest.xlsx
+++ b/DataValidation/test-files/DataValidationTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>Any Value</t>
   </si>
@@ -111,12 +111,48 @@
     <t>Ahmet, Mehmet, Süleyman</t>
   </si>
   <si>
+    <t>Case 19</t>
+  </si>
+  <si>
     <t>Case 20</t>
   </si>
   <si>
     <t>Case 21</t>
   </si>
   <si>
+    <t>Case 22</t>
+  </si>
+  <si>
+    <t>Case 23</t>
+  </si>
+  <si>
+    <t>Case 24</t>
+  </si>
+  <si>
+    <t>Case 25</t>
+  </si>
+  <si>
+    <t>Case 26</t>
+  </si>
+  <si>
+    <t>Case 27</t>
+  </si>
+  <si>
+    <t>Case 28</t>
+  </si>
+  <si>
+    <t>Case 29</t>
+  </si>
+  <si>
+    <t>Case 30</t>
+  </si>
+  <si>
+    <t>Case 31</t>
+  </si>
+  <si>
+    <t>Case 32</t>
+  </si>
+  <si>
     <t>Case 33</t>
   </si>
   <si>
@@ -132,6 +168,9 @@
     <t>-</t>
   </si>
   <si>
+    <t>"Ahmet, Mehmet, Süleyman"</t>
+  </si>
+  <si>
     <t>Ref1</t>
   </si>
   <si>
@@ -159,6 +198,15 @@
     <t>Ref4!</t>
   </si>
   <si>
+    <t>J1:J3</t>
+  </si>
+  <si>
+    <t>K1:K3</t>
+  </si>
+  <si>
+    <t>L1:L3</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -174,29 +222,105 @@
     <t>Case 41</t>
   </si>
   <si>
-    <t>Yusuf</t>
-  </si>
-  <si>
-    <t>RefS4!</t>
+    <t>E33</t>
+  </si>
+  <si>
+    <t>F33</t>
+  </si>
+  <si>
+    <t>E34</t>
+  </si>
+  <si>
+    <t>F34</t>
+  </si>
+  <si>
+    <t>E35</t>
+  </si>
+  <si>
+    <t>E36</t>
+  </si>
+  <si>
+    <t>E37</t>
+  </si>
+  <si>
+    <t>E38</t>
+  </si>
+  <si>
+    <t>E39</t>
+  </si>
+  <si>
+    <t>E40</t>
+  </si>
+  <si>
+    <t>Case 42</t>
+  </si>
+  <si>
+    <t>Case 43</t>
+  </si>
+  <si>
+    <t>Case 44</t>
+  </si>
+  <si>
+    <t>Case 45</t>
+  </si>
+  <si>
+    <t>Case 46</t>
+  </si>
+  <si>
+    <t>Case 47</t>
+  </si>
+  <si>
+    <t>Case 48</t>
+  </si>
+  <si>
+    <t>Case 49</t>
+  </si>
+  <si>
+    <t>Case 50</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Text Length</t>
+  </si>
+  <si>
+    <t>E44</t>
+  </si>
+  <si>
+    <t>F44</t>
+  </si>
+  <si>
+    <t>Sheet2# E1</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>H49</t>
+  </si>
+  <si>
+    <t>H50</t>
+  </si>
+  <si>
+    <t>Case 34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="d/m/yyyy\ hh:mm;@"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy\ hh:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -223,12 +347,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,9 +369,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Ofis">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -284,7 +409,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Ofis">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -356,7 +481,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Ofis">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +668,7 @@
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" customWidth="1"/>
   </cols>
@@ -556,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="J1">
         <v>12</v>
@@ -575,10 +700,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
@@ -591,7 +713,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="J2">
         <v>14</v>
@@ -610,9 +732,6 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
@@ -626,7 +745,7 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="J3">
         <v>16</v>
@@ -642,9 +761,6 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
@@ -655,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="J4">
         <v>18</v>
@@ -665,9 +781,6 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
@@ -682,9 +795,6 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
@@ -699,9 +809,6 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>888</v>
-      </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
@@ -716,9 +823,6 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
@@ -733,9 +837,6 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
-        <v>888</v>
-      </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
@@ -750,9 +851,6 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>15</v>
-      </c>
       <c r="C10" t="s">
         <v>28</v>
       </c>
@@ -770,9 +868,6 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>2.2200000000000002</v>
-      </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
@@ -790,9 +885,6 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>15</v>
-      </c>
       <c r="C12" t="s">
         <v>28</v>
       </c>
@@ -807,9 +899,6 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
-        <v>6.66</v>
-      </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
@@ -824,9 +913,6 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
       <c r="C14" t="s">
         <v>28</v>
       </c>
@@ -841,9 +927,6 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
-        <v>1000</v>
-      </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
@@ -858,9 +941,6 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
       <c r="C16" t="s">
         <v>28</v>
       </c>
@@ -871,13 +951,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
-        <v>1000</v>
-      </c>
       <c r="C17" t="s">
         <v>28</v>
       </c>
@@ -888,201 +965,492 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
       <c r="C18" t="s">
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
       <c r="C19" t="s">
         <v>29</v>
       </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
       <c r="E19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
       <c r="C20" t="s">
         <v>29</v>
       </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
       <c r="E20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="2">
-        <v>42005</v>
-      </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2">
-        <v>42343</v>
-      </c>
-      <c r="F21" s="2">
-        <v>42710</v>
-      </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="2">
-        <v>42343</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>47</v>
+      <c r="C22" t="s">
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="2">
-        <v>42343</v>
-      </c>
-      <c r="F22" s="2">
-        <v>42710</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="2">
-        <v>42370</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
+      <c r="C23" t="s">
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="2">
-        <v>42343</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="2">
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="2">
         <v>42343</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="F33" s="2">
+        <v>42710</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="2">
+        <v>42343</v>
+      </c>
+      <c r="F34" s="2">
+        <v>42710</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>47</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E36" s="2">
         <v>42343</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2">
+      <c r="C37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="2">
         <v>42343</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="2">
-        <v>42343</v>
-      </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2">
-        <v>42370</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="2">
-        <v>42343</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="2">
-        <v>42340</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="2">
-        <v>42343</v>
-      </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="2">
-        <v>42370</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="2">
-        <v>42343</v>
+      <c r="E46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H49" s="4">
+        <v>41975.541666666664</v>
+      </c>
+      <c r="I49" s="4">
+        <v>41975.708333333336</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="25">
+  <dataValidations count="44">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>1</formula1>
       <formula2>10</formula2>
@@ -1100,6 +1468,9 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>7</formula1>
     </dataValidation>
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>111</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>65</formula1>
     </dataValidation>
@@ -1136,45 +1507,111 @@
       <formula1>"Ahmet,Mehmet,Süleyman"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
+      <formula1>"""Ahmet,Mehmet,Süleyman"""</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
       <formula1>$I$1:$I$3</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+      <formula1>$J$1:$J$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
+      <formula1>$K$1:$K$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+      <formula1>$L$1:$L$3</formula1>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
       <formula1>42343</formula1>
       <formula2>42710</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+      <formula1>E33</formula1>
+      <formula2>F33</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
       <formula1>42343</formula1>
       <formula2>42710</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
+    <dataValidation type="date" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
       <formula1>42343</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B25">
+    <dataValidation type="date" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:B37">
       <formula1>42343</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
+    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
       <formula1>42343</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
       <formula1>42343</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
       <formula1>42343</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
-      <formula1>111</formula1>
+    <dataValidation type="date" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
+      <formula1>E34</formula1>
+      <formula2>F34</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
+      <formula1>E35</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+      <formula1>E36</formula1>
+    </dataValidation>
+    <dataValidation type="time" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29">
+      <formula1>E37</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
+      <formula1>E38</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
+      <formula1>E39</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
+      <formula1>E40</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41">
+      <formula1>E2</formula1>
+      <formula2>F2</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
+      <formula1>E10</formula1>
+      <formula2>F10</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43">
+      <formula1>E17</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45">
+      <formula1>E44</formula1>
+      <formula2>F44</formula2>
+    </dataValidation>
+    <dataValidation type="time" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48">
+      <formula1>H49</formula1>
+    </dataValidation>
+    <dataValidation type="time" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50">
+      <formula1>H49</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sayfa2!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B20</xm:sqref>
+          <xm:sqref>B21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sayfa2!E1</xm:f>
+          </x14:formula1>
+          <xm:sqref>B47</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1184,32 +1621,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:C4"/>
+  <dimension ref="C1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>